<commit_message>
Update prism templates for capture tun time
</commit_message>
<xml_diff>
--- a/Template/EC_Template.xlsx
+++ b/Template/EC_Template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t xml:space="preserve">Exact Cover</t>
   </si>
@@ -71,13 +71,16 @@
     <t xml:space="preserve">CTL Runtime (ms)</t>
   </si>
   <si>
-    <t xml:space="preserve">Prism No Tag File Name</t>
+    <t xml:space="preserve">Prism File Name</t>
   </si>
   <si>
     <t xml:space="preserve">EC Exists with mu=0</t>
   </si>
   <si>
     <t xml:space="preserve">Prob for EC with mu=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runtime (ms)</t>
   </si>
   <si>
     <t xml:space="preserve">EC Exists with mu</t>
@@ -345,20 +348,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
+      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="7.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="13.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="13.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -373,6 +377,8 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -401,6 +407,12 @@
       </c>
       <c r="I2" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -413,11 +425,12 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A1:I1"/>
+  <mergeCells count="12">
+    <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -427,6 +440,8 @@
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>